<commit_message>
Fixing network data cleanining scripts
</commit_message>
<xml_diff>
--- a/Data_clean/MCAS/Estados_US/Edos_USA_2010/MAINE_2010.xlsx
+++ b/Data_clean/MCAS/Estados_US/Edos_USA_2010/MAINE_2010.xlsx
@@ -360,45 +360,41 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Estado de Origen</t>
+          <t>mx_state</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Municipio de Origen</t>
+          <t>mx_municipality</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Número de Matrículas</t>
+          <t>n_matriculas</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Porcentaje de Matrículas</t>
+          <t>pct_matriculas</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BAJA CALIFORNIA</t>
+          <t>Baja California</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TIJUANA</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Tijuana</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="3">
@@ -407,37 +403,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHIAPAS</t>
+          <t>Chiapas</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>HUEHUETAN</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Huehuetan</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="5">
@@ -446,37 +434,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CHIHUAHUA</t>
+          <t>Chihuahua</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>JUAREZ</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Juarez</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="7">
@@ -485,71 +465,55 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>COLIMA</t>
+          <t>Colima</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>COLIMA</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Colima</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>MANZANILLO</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Manzanillo</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>MINATITLAN</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>5.2600000000000001E-2</t>
-        </is>
+          <t>Minatitlan</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0.0526</v>
       </c>
     </row>
     <row r="11">
@@ -558,37 +522,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.1053</t>
-        </is>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0.1053</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DISTRITO FEDERAL</t>
+          <t>Distrito Federal</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GUSTAVO A. MADERO</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>5.2600000000000001E-2</t>
-        </is>
+          <t>Gustavo A. Madero</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0.0526</v>
       </c>
     </row>
     <row r="13">
@@ -597,71 +553,55 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5.2600000000000001E-2</t>
-        </is>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0.0526</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GUANAJUATO</t>
+          <t>Guanajuato</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CELAYA</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Celaya</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>TARIMORO</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>7.8899999999999998E-2</t>
-        </is>
+          <t>Tarimoro</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0.0789</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>VALLE DE SANTIAGO</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Valle De Santiago</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="17">
@@ -670,37 +610,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0.13159999999999999</t>
-        </is>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0.1316</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>JALISCO</t>
+          <t>Jalisco</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IXTLAHUACAN DEL RIO</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Ixtlahuacan Del Rio</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="19">
@@ -709,37 +641,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MEXICO</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IXTLAHUACA</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>5.2600000000000001E-2</t>
-        </is>
+          <t>Ixtlahuaca</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>0.0526</v>
       </c>
     </row>
     <row r="21">
@@ -748,54 +672,42 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>5.2600000000000001E-2</t>
-        </is>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>0.0526</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MICHOACAN DE OCAMPO</t>
+          <t>Michoacan De Ocampo</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LAZARO CARDENAS</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Lazaro Cardenas</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>MORELIA</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>7.8899999999999998E-2</t>
-        </is>
+          <t>Morelia</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>0.0789</v>
       </c>
     </row>
     <row r="24">
@@ -804,71 +716,55 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0.1053</t>
-        </is>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>0.1053</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>OAXACA</t>
+          <t>Oaxaca</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OAXACA DE JUAREZ</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>7.8899999999999998E-2</t>
-        </is>
+          <t>Oaxaca De Juarez</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>0.0789</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>SANTO DOMINGO TOMALTEPEC</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Santo Domingo Tomaltepec</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>VILLA DE CHILAPA DE DIAZ</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Villa De Chilapa De Diaz</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="28">
@@ -877,105 +773,81 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>0.13159999999999999</t>
-        </is>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>0.1316</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PUEBLA</t>
+          <t>Puebla</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ATLIXCO</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Atlixco</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>HUAQUECHULA</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Huaquechula</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>PUEBLA</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>5.2600000000000001E-2</t>
-        </is>
+          <t>Puebla</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>0.0526</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>SAN ANDRES CHOLULA</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>San Andres Cholula</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>TEZIUTLAN</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Teziutlan</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="34">
@@ -984,37 +856,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0.15790000000000001</t>
-        </is>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>0.1579</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SAN LUIS POTOSI</t>
+          <t>San Luis Potosi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CIUDAD DEL MAIZ</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>0.1053</t>
-        </is>
+          <t>Ciudad Del Maiz</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>0.1053</v>
       </c>
     </row>
     <row r="36">
@@ -1023,37 +887,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>0.1053</t>
-        </is>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>0.1053</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>VERACRUZ DE IGNACIO DE LA LLAVE</t>
+          <t>Veracruz De Ignacio De La Llave</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MINATITLAN</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Minatitlan</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="38">
@@ -1062,37 +918,29 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ZACATECAS</t>
+          <t>Zacatecas</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CHALCHIHUITES</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+          <t>Chalchihuites</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="40">
@@ -1101,21 +949,17 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>2.63E-2</t>
-        </is>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.0263</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TOTAL</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1123,15 +967,11 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C41">
+        <v>38</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>